<commit_message>
incorporated sus score in presentation
</commit_message>
<xml_diff>
--- a/sus/sus_questionnaire.xlsx
+++ b/sus/sus_questionnaire.xlsx
@@ -1,22 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="96" yWindow="84" windowWidth="13380" windowHeight="4008"/>
+    <workbookView xWindow="90" yWindow="90" windowWidth="7335" windowHeight="4005" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Joris Klerkx" sheetId="1" r:id="rId1"/>
     <sheet name="Erik Duval" sheetId="2" r:id="rId2"/>
     <sheet name="Niels Billen" sheetId="3" r:id="rId3"/>
+    <sheet name="Niels Keyword" sheetId="4" r:id="rId4"/>
+    <sheet name="Stijn" sheetId="5" r:id="rId5"/>
+    <sheet name="Stijn keyword" sheetId="6" r:id="rId6"/>
+    <sheet name="Robin" sheetId="7" r:id="rId7"/>
+    <sheet name="Robin Keyword" sheetId="8" r:id="rId8"/>
+    <sheet name="Erik Duval Keywordmap" sheetId="9" r:id="rId9"/>
+    <sheet name="Blad7" sheetId="10" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="22">
   <si>
     <t>I think that I would like to use this system frequently.</t>
   </si>
@@ -55,13 +62,40 @@
   </si>
   <si>
     <t>SUS questionnaire capsel visualization</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Keywordmap</t>
+  </si>
+  <si>
+    <t>switchinglakmap</t>
+  </si>
+  <si>
+    <t>Person</t>
+  </si>
+  <si>
+    <t>Niels</t>
+  </si>
+  <si>
+    <t>Robin</t>
+  </si>
+  <si>
+    <t>Stijn</t>
+  </si>
+  <si>
+    <t>Average</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -103,7 +137,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -116,9 +150,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-thema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Kantoor">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -156,7 +190,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Kantoor">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -190,7 +224,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -225,10 +258,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Kantoor">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -401,26 +433,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="73.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" customWidth="1"/>
+    <col min="1" max="1" width="73.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" ht="23.25">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6">
       <c r="B2" t="s">
         <v>10</v>
       </c>
@@ -428,7 +460,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6">
       <c r="B3">
         <v>1</v>
       </c>
@@ -445,52 +477,52 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -501,25 +533,101 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2">
+        <v>80</v>
+      </c>
+      <c r="C2">
+        <v>77.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3">
+        <v>82.5</v>
+      </c>
+      <c r="C3">
+        <v>82.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4">
+        <v>90</v>
+      </c>
+      <c r="C4">
+        <v>82.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5">
+        <f>AVERAGE(B2:B4)</f>
+        <v>84.166666666666671</v>
+      </c>
+      <c r="C5">
+        <f>AVERAGE(C2:C4)</f>
+        <v>80.833333333333329</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="73.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="80.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" ht="23.25">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6">
       <c r="B2" t="s">
         <v>10</v>
       </c>
@@ -527,7 +635,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6">
       <c r="B3">
         <v>1</v>
       </c>
@@ -544,52 +652,52 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -600,24 +708,1054 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="80.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="23.25">
+      <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>4</v>
+      </c>
+      <c r="F3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="G14">
+        <f>SUM(G4:G13)</f>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="G15">
+        <f>G14*2.5</f>
+        <v>77.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="80.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="23.25">
+      <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>4</v>
+      </c>
+      <c r="F3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="G14">
+        <f>SUM(G4:G13)</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="G15">
+        <f>G14*2.5</f>
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G14" sqref="G14:G16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="80.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="23.25">
+      <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>4</v>
+      </c>
+      <c r="F3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="G14">
+        <f>SUM(G4:G13)</f>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="G15">
+        <f>G14*2.5</f>
+        <v>82.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="80.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" customWidth="1"/>
+    <col min="3" max="3" width="6" customWidth="1"/>
+    <col min="4" max="4" width="7.7109375" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="23.25">
+      <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>4</v>
+      </c>
+      <c r="F3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="G14">
+        <f>SUM(G4:G13)</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="G15">
+        <f>G14*2.5</f>
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="80.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="23.25">
+      <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>4</v>
+      </c>
+      <c r="F3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="G14">
+        <f>SUM(G4:G13)</f>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="G15">
+        <f>G14*2.5</f>
+        <v>82.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="73.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="23.25">
+      <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>4</v>
+      </c>
+      <c r="F3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="G14">
+        <f>SUM(G4:G13)</f>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="G15">
+        <f>G14*2.5</f>
+        <v>82.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:I18"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="73.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="80.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" ht="23.25">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6">
       <c r="B2" t="s">
         <v>10</v>
       </c>
@@ -625,7 +1763,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6">
       <c r="B3">
         <v>1</v>
       </c>
@@ -642,52 +1780,52 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>9</v>
       </c>

</xml_diff>